<commit_message>
add print best model
</commit_message>
<xml_diff>
--- a/likelihood_formulas_M1.xlsx
+++ b/likelihood_formulas_M1.xlsx
@@ -567,31 +567,31 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.2045</v>
+        <v>1.078</v>
       </c>
       <c r="E2">
         <v>787</v>
       </c>
       <c r="F2">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G2">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H2">
-        <v>547.3623143800562</v>
+        <v>480.4315793651584</v>
       </c>
       <c r="I2">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J2">
-        <v>0.2029972392006026</v>
+        <v>0.2218081509276456</v>
       </c>
       <c r="K2">
-        <v>0.0007814619150194428</v>
+        <v>0.0003693002306110245</v>
       </c>
       <c r="L2">
-        <v>7.931730564468138E-05</v>
+        <v>4.095690064449222E-05</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -602,34 +602,34 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-0.866</v>
+        <v>-0.158</v>
       </c>
       <c r="E3">
         <v>605.67</v>
       </c>
       <c r="F3">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G3">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H3">
-        <v>479.676224351104</v>
+        <v>517.4379985492587</v>
       </c>
       <c r="I3">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J3">
-        <v>0.2645782773934067</v>
+        <v>0.4494943539283914</v>
       </c>
       <c r="K3">
-        <v>0.00184825568401154</v>
+        <v>0.002181461462784426</v>
       </c>
       <c r="L3">
-        <v>0.0002445041525291729</v>
+        <v>0.0004902773054169847</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -643,31 +643,31 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.7865</v>
+        <v>0.8565</v>
       </c>
       <c r="E4">
         <v>566</v>
       </c>
       <c r="F4">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G4">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H4">
-        <v>533.697602652405</v>
+        <v>487.0633931590728</v>
       </c>
       <c r="I4">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J4">
-        <v>0.3334030436882156</v>
+        <v>0.2923483315652065</v>
       </c>
       <c r="K4">
-        <v>0.00251304926141707</v>
+        <v>0.002252437998901005</v>
       </c>
       <c r="L4">
-        <v>0.0004189291363474366</v>
+        <v>0.0003292482454663905</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -678,34 +678,34 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.9525</v>
+        <v>-0.7004999999999999</v>
       </c>
       <c r="E5">
         <v>361.23</v>
       </c>
       <c r="F5">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G5">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H5">
-        <v>539.1242585059698</v>
+        <v>533.6807027623447</v>
       </c>
       <c r="I5">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J5">
-        <v>0.266773069370445</v>
+        <v>0.322462101258693</v>
       </c>
       <c r="K5">
-        <v>0.00133308269454928</v>
+        <v>0.001387667903401309</v>
       </c>
       <c r="L5">
-        <v>0.0001778152810747674</v>
+        <v>0.0002237351539900155</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -719,31 +719,31 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>-0.873</v>
+        <v>0.2875</v>
       </c>
       <c r="E6">
         <v>572.5</v>
       </c>
       <c r="F6">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G6">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H6">
-        <v>479.4473894657127</v>
+        <v>504.099519789941</v>
       </c>
       <c r="I6">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J6">
-        <v>0.2477472043680699</v>
+        <v>0.4405081015324698</v>
       </c>
       <c r="K6">
-        <v>0.002146265343594602</v>
+        <v>0.002325650238842761</v>
       </c>
       <c r="L6">
-        <v>0.0002658656193538189</v>
+        <v>0.0005122338857705799</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -754,34 +754,34 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.2875</v>
+        <v>-0.9385</v>
       </c>
       <c r="E7">
         <v>515.6</v>
       </c>
       <c r="F7">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G7">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H7">
-        <v>517.3849443937972</v>
+        <v>540.8065342880858</v>
       </c>
       <c r="I7">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J7">
-        <v>0.4398039512531491</v>
+        <v>0.2463224265731103</v>
       </c>
       <c r="K7">
-        <v>0.002567796075982972</v>
+        <v>0.002527703384733456</v>
       </c>
       <c r="L7">
-        <v>0.0005646634301148212</v>
+        <v>0.0003113150156923045</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -795,31 +795,31 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1.175</v>
+        <v>-0.885</v>
       </c>
       <c r="E8">
         <v>524.11</v>
       </c>
       <c r="F8">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G8">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H8">
-        <v>546.3979387916215</v>
+        <v>539.2047192182238</v>
       </c>
       <c r="I8">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J8">
-        <v>0.2118214453195885</v>
+        <v>0.2634218459225235</v>
       </c>
       <c r="K8">
-        <v>0.002541673517716769</v>
+        <v>0.002549017726631687</v>
       </c>
       <c r="L8">
-        <v>0.0002691904790266444</v>
+        <v>0.0003357334774192768</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -830,34 +830,34 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.8565</v>
+        <v>0.5565</v>
       </c>
       <c r="E9">
         <v>487.4</v>
       </c>
       <c r="F9">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G9">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H9">
-        <v>535.9859515063179</v>
+        <v>496.045533737738</v>
       </c>
       <c r="I9">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J9">
-        <v>0.3117742692165829</v>
+        <v>0.4080401550507186</v>
       </c>
       <c r="K9">
-        <v>0.002445401642649875</v>
+        <v>0.002557071915048779</v>
       </c>
       <c r="L9">
-        <v>0.000381206655039098</v>
+        <v>0.0005216940103461708</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -871,31 +871,31 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>-0.158</v>
+        <v>-1.0935</v>
       </c>
       <c r="E10">
         <v>603.33</v>
       </c>
       <c r="F10">
-        <v>0.0467142857142857</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G10">
-        <v>0.7625757040816327</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H10">
-        <v>502.8212384735373</v>
+        <v>545.447306920396</v>
       </c>
       <c r="I10">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J10">
-        <v>0.4444624631343972</v>
+        <v>0.1669372924942746</v>
       </c>
       <c r="K10">
-        <v>0.0020830432779051</v>
+        <v>0.002390177644376891</v>
       </c>
       <c r="L10">
-        <v>0.0004629172730566248</v>
+        <v>0.0001995048922663107</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -909,31 +909,31 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>-0.886</v>
+        <v>-0.6830000000000001</v>
       </c>
       <c r="E11">
         <v>389</v>
       </c>
       <c r="F11">
-        <v>0.0467142857142857</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G11">
-        <v>0.7625757040816327</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H11">
-        <v>479.0224103928432</v>
+        <v>533.1567445619227</v>
       </c>
       <c r="I11">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J11">
-        <v>0.2582523513871741</v>
+        <v>0.2900953660141034</v>
       </c>
       <c r="K11">
-        <v>0.002171074392855872</v>
+        <v>0.001668969113411414</v>
       </c>
       <c r="L11">
-        <v>0.0002803425334957552</v>
+        <v>0.0002420801029106588</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -947,31 +947,31 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>-0.8935</v>
+        <v>1.175</v>
       </c>
       <c r="E12">
         <v>664</v>
       </c>
       <c r="F12">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G12">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H12">
-        <v>478.7772301584954</v>
+        <v>477.52735391139</v>
       </c>
       <c r="I12">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J12">
-        <v>0.2413135221868268</v>
+        <v>0.1925442100805093</v>
       </c>
       <c r="K12">
-        <v>0.001261578530625077</v>
+        <v>0.001250975264108357</v>
       </c>
       <c r="L12">
-        <v>0.0001522179793702095</v>
+        <v>0.0001204340220290001</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -982,34 +982,34 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>-0.776</v>
+        <v>-0.8155</v>
       </c>
       <c r="E13">
         <v>467</v>
       </c>
       <c r="F13">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G13">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H13">
-        <v>482.6183871632778</v>
+        <v>537.1238566508331</v>
       </c>
       <c r="I13">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J13">
-        <v>0.2784992428694513</v>
+        <v>0.2485770863875782</v>
       </c>
       <c r="K13">
-        <v>0.002555020841601338</v>
+        <v>0.002314238379455394</v>
       </c>
       <c r="L13">
-        <v>0.0003557856849508205</v>
+        <v>0.0002876333167856663</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1020,34 +1020,34 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.9165</v>
+        <v>-0.873</v>
       </c>
       <c r="E14">
         <v>564</v>
       </c>
       <c r="F14">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G14">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H14">
-        <v>537.9473933811004</v>
+        <v>538.8454335950772</v>
       </c>
       <c r="I14">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J14">
-        <v>0.292849904090963</v>
+        <v>0.2308190165259935</v>
       </c>
       <c r="K14">
-        <v>0.002532108895893462</v>
+        <v>0.002527839699077095</v>
       </c>
       <c r="L14">
-        <v>0.0003707639236551372</v>
+        <v>0.0002917367366381693</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1061,31 +1061,31 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.619</v>
+        <v>1.0325</v>
       </c>
       <c r="E15">
         <v>484.19</v>
       </c>
       <c r="F15">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G15">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H15">
-        <v>528.2219107519705</v>
+        <v>481.793870686256</v>
       </c>
       <c r="I15">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J15">
-        <v>0.381340216058528</v>
+        <v>0.236007876722867</v>
       </c>
       <c r="K15">
-        <v>0.002466863582807173</v>
+        <v>0.002560710213667116</v>
       </c>
       <c r="L15">
-        <v>0.0004703571458273009</v>
+        <v>0.0003021738902150675</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1096,34 +1096,34 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0.6525000000000001</v>
+        <v>-0.8335</v>
       </c>
       <c r="E16">
         <v>672.08</v>
       </c>
       <c r="F16">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G16">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H16">
-        <v>529.3170491320574</v>
+        <v>537.662785085553</v>
       </c>
       <c r="I16">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J16">
-        <v>0.3591453435957837</v>
+        <v>0.279992869259803</v>
       </c>
       <c r="K16">
-        <v>0.001683498470319609</v>
+        <v>0.001764930497934621</v>
       </c>
       <c r="L16">
-        <v>0.0003023103182829561</v>
+        <v>0.0002470839770804236</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1137,31 +1137,31 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>-1.086</v>
+        <v>0.7865</v>
       </c>
       <c r="E17">
         <v>664.8</v>
       </c>
       <c r="F17">
-        <v>0.0467142857142857</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G17">
-        <v>0.7625757040816327</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H17">
-        <v>472.4842708102349</v>
+        <v>489.1592259607614</v>
       </c>
       <c r="I17">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J17">
-        <v>0.1969772472354962</v>
+        <v>0.349081822036577</v>
       </c>
       <c r="K17">
-        <v>0.00119349529698072</v>
+        <v>0.001356277721552651</v>
       </c>
       <c r="L17">
-        <v>0.0001175457090938866</v>
+        <v>0.0002367259491136083</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1175,31 +1175,31 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0.9590000000000001</v>
+        <v>0.6525000000000001</v>
       </c>
       <c r="E18">
         <v>533</v>
       </c>
       <c r="F18">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G18">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H18">
-        <v>539.3367480424046</v>
+        <v>493.1712487525651</v>
       </c>
       <c r="I18">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J18">
-        <v>0.279343096182044</v>
+        <v>0.3558436928339854</v>
       </c>
       <c r="K18">
-        <v>0.002565830216110049</v>
+        <v>0.002478656218349355</v>
       </c>
       <c r="L18">
-        <v>0.0003583734784228121</v>
+        <v>0.0004410070910016778</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1210,34 +1210,34 @@
         <v>28</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1.0325</v>
+        <v>0.7185</v>
       </c>
       <c r="E19">
         <v>695.67</v>
       </c>
       <c r="F19">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G19">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H19">
-        <v>541.7395143390131</v>
+        <v>491.1951778252588</v>
       </c>
       <c r="I19">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J19">
-        <v>0.2415745796754493</v>
+        <v>0.3359509427485166</v>
       </c>
       <c r="K19">
-        <v>0.001571815756008834</v>
+        <v>0.001082103821852518</v>
       </c>
       <c r="L19">
-        <v>0.0001898553652925413</v>
+        <v>0.0001817668995515631</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1251,31 +1251,31 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>-0.8195</v>
+        <v>-0.886</v>
       </c>
       <c r="E20">
         <v>437</v>
       </c>
       <c r="F20">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G20">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H20">
-        <v>481.1963418040605</v>
+        <v>539.2346596868193</v>
       </c>
       <c r="I20">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J20">
-        <v>0.2646672831718254</v>
+        <v>0.2631007852535654</v>
       </c>
       <c r="K20">
-        <v>0.002466122273162796</v>
+        <v>0.002064814902412787</v>
       </c>
       <c r="L20">
-        <v>0.0003263509410037617</v>
+        <v>0.0002716272111140341</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1289,31 +1289,31 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>-0.6830000000000001</v>
+        <v>-1.1685</v>
       </c>
       <c r="E21">
         <v>765.75</v>
       </c>
       <c r="F21">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G21">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H21">
-        <v>485.6586220691906</v>
+        <v>547.6928420650623</v>
       </c>
       <c r="I21">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J21">
-        <v>0.3079628210145719</v>
+        <v>0.1767454715857837</v>
       </c>
       <c r="K21">
-        <v>0.0005055216787071028</v>
+        <v>0.0009614193358772819</v>
       </c>
       <c r="L21">
-        <v>7.78409411293307E-05</v>
+        <v>8.496325695566056E-05</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1324,34 +1324,34 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0.7595000000000001</v>
+        <v>1.2175</v>
       </c>
       <c r="E22">
         <v>637.25</v>
       </c>
       <c r="F22">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G22">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H22">
-        <v>532.8149538087529</v>
+        <v>476.2548839960791</v>
       </c>
       <c r="I22">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J22">
-        <v>0.341552376510002</v>
+        <v>0.216580217538293</v>
       </c>
       <c r="K22">
-        <v>0.002048606044783715</v>
+        <v>0.001501301006003333</v>
       </c>
       <c r="L22">
-        <v>0.0003498531315643166</v>
+        <v>0.00016257604923533</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1362,34 +1362,34 @@
         <v>32</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0.899</v>
+        <v>-1.086</v>
       </c>
       <c r="E23">
         <v>819</v>
       </c>
       <c r="F23">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G23">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H23">
-        <v>537.3753061676221</v>
+        <v>545.2227534059294</v>
       </c>
       <c r="I23">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J23">
-        <v>0.2837429863771165</v>
+        <v>0.2007121328136323</v>
       </c>
       <c r="K23">
-        <v>0.0004965814698674819</v>
+        <v>0.0005466060460966369</v>
       </c>
       <c r="L23">
-        <v>7.045075461986871E-05</v>
+        <v>5.48552326604413E-05</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1403,31 +1403,31 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0.8125</v>
+        <v>-0.8205</v>
       </c>
       <c r="E24">
         <v>665</v>
       </c>
       <c r="F24">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G24">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H24">
-        <v>534.547560798144</v>
+        <v>537.2735589938108</v>
       </c>
       <c r="I24">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J24">
-        <v>0.3254443742683569</v>
+        <v>0.2841794770206726</v>
       </c>
       <c r="K24">
-        <v>0.001804988595579666</v>
+        <v>0.001829881845442532</v>
       </c>
       <c r="L24">
-        <v>0.0002937116920249723</v>
+        <v>0.0002600074329237411</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1438,34 +1438,34 @@
         <v>34</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.7185</v>
+        <v>0.7595000000000001</v>
       </c>
       <c r="E25">
         <v>334.75</v>
       </c>
       <c r="F25">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G25">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H25">
-        <v>531.4746351943181</v>
+        <v>489.9676186128412</v>
       </c>
       <c r="I25">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J25">
-        <v>0.3536609159170859</v>
+        <v>0.3568029592621747</v>
       </c>
       <c r="K25">
-        <v>0.001151829369981377</v>
+        <v>0.001558892753899175</v>
       </c>
       <c r="L25">
-        <v>0.0002036785149839069</v>
+        <v>0.0002781087738817933</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1476,34 +1476,34 @@
         <v>35</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>-0.885</v>
+        <v>-0.776</v>
       </c>
       <c r="E26">
         <v>307.83</v>
       </c>
       <c r="F26">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G26">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H26">
-        <v>479.0551010907562</v>
+        <v>535.9412081413088</v>
       </c>
       <c r="I26">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J26">
-        <v>0.2439769800359151</v>
+        <v>0.26091190353275</v>
       </c>
       <c r="K26">
-        <v>0.001398961652263236</v>
+        <v>0.0008765384658680946</v>
       </c>
       <c r="L26">
-        <v>0.0001706572195526192</v>
+        <v>0.0001143496598246605</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1514,34 +1514,34 @@
         <v>36</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>1.078</v>
+        <v>0.9590000000000001</v>
       </c>
       <c r="E27">
         <v>442</v>
       </c>
       <c r="F27">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G27">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H27">
-        <v>543.2269410940565</v>
+        <v>483.9944951280289</v>
       </c>
       <c r="I27">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J27">
-        <v>0.2274664472746304</v>
+        <v>0.2593769358155739</v>
       </c>
       <c r="K27">
-        <v>0.002076800314974719</v>
+        <v>0.002469622200422008</v>
       </c>
       <c r="L27">
-        <v>0.0002362011946730664</v>
+        <v>0.0003202815194837877</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1552,34 +1552,34 @@
         <v>37</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1.2175</v>
+        <v>-0.8935</v>
       </c>
       <c r="E28">
         <v>260.42</v>
       </c>
       <c r="F28">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G28">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H28">
-        <v>547.7872934529258</v>
+        <v>539.4592132012859</v>
       </c>
       <c r="I28">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J28">
-        <v>0.1859703688796758</v>
+        <v>0.2606942091909677</v>
       </c>
       <c r="K28">
-        <v>0.0004640789479537661</v>
+        <v>0.0005148060835807066</v>
       </c>
       <c r="L28">
-        <v>4.315246657012687E-05</v>
+        <v>6.710348242288576E-05</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1590,34 +1590,34 @@
         <v>38</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>-0.9385</v>
+        <v>1.2045</v>
       </c>
       <c r="E29">
         <v>448.82</v>
       </c>
       <c r="F29">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G29">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H29">
-        <v>477.3061487524085</v>
+        <v>476.6441100878213</v>
       </c>
       <c r="I29">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J29">
-        <v>0.2273296794601091</v>
+        <v>0.220497362994497</v>
       </c>
       <c r="K29">
-        <v>0.002525156126868006</v>
+        <v>0.002520483922708827</v>
       </c>
       <c r="L29">
-        <v>0.0002870214664538172</v>
+        <v>0.000277880029213661</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1631,31 +1631,31 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>-0.8205</v>
+        <v>0.8034999999999999</v>
       </c>
       <c r="E30">
         <v>455.38</v>
       </c>
       <c r="F30">
-        <v>0.0467142857142857</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G30">
-        <v>0.7625757040816327</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H30">
-        <v>481.1636511061474</v>
+        <v>488.650237994637</v>
       </c>
       <c r="I30">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J30">
-        <v>0.2790072998467366</v>
+        <v>0.3441392028744556</v>
       </c>
       <c r="K30">
-        <v>0.00253284035062869</v>
+        <v>0.002503262920684621</v>
       </c>
       <c r="L30">
-        <v>0.0003533404735858862</v>
+        <v>0.0004307354530547935</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1666,34 +1666,34 @@
         <v>40</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>-0.8155</v>
+        <v>0.7985</v>
       </c>
       <c r="E31">
         <v>89.5</v>
       </c>
       <c r="F31">
-        <v>0.0467142857142857</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G31">
-        <v>0.7625757040816327</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H31">
-        <v>481.3271045957126</v>
+        <v>488.7999403376148</v>
       </c>
       <c r="I31">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J31">
-        <v>0.2805936789492554</v>
+        <v>0.3108972592602556</v>
       </c>
       <c r="K31">
-        <v>0.0001067200967055567</v>
+        <v>9.58592793475536E-05</v>
       </c>
       <c r="L31">
-        <v>1.497249227621623E-05</v>
+        <v>1.490119361190882E-05</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1707,31 +1707,31 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>-0.8335</v>
+        <v>0.899</v>
       </c>
       <c r="E32">
         <v>437.64</v>
       </c>
       <c r="F32">
-        <v>0.0467142857142857</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G32">
-        <v>0.7625757040816327</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H32">
-        <v>480.7386720332779</v>
+        <v>485.7909232437619</v>
       </c>
       <c r="I32">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J32">
-        <v>0.2748823841533381</v>
+        <v>0.3154388776041464</v>
       </c>
       <c r="K32">
-        <v>0.002471022714006059</v>
+        <v>0.002441542289870729</v>
       </c>
       <c r="L32">
-        <v>0.0003396203074615188</v>
+        <v>0.0003850786797699401</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1745,31 +1745,31 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>0.7985</v>
+        <v>0.619</v>
       </c>
       <c r="E33">
         <v>354</v>
       </c>
       <c r="F33">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G33">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H33">
-        <v>534.0898910273614</v>
+        <v>494.1742544505161</v>
       </c>
       <c r="I33">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J33">
-        <v>0.3297423314034877</v>
+        <v>0.3655752487057839</v>
       </c>
       <c r="K33">
-        <v>0.001311551027385802</v>
+        <v>0.001708367374011152</v>
       </c>
       <c r="L33">
-        <v>0.000216236946762417</v>
+        <v>0.0003122684138174869</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1783,31 +1783,31 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>-1.1685</v>
+        <v>-0.866</v>
       </c>
       <c r="E34">
         <v>605</v>
       </c>
       <c r="F34">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G34">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H34">
-        <v>469.787288232409</v>
+        <v>538.6358503149083</v>
       </c>
       <c r="I34">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J34">
-        <v>0.1607264882485248</v>
+        <v>0.2695288113114986</v>
       </c>
       <c r="K34">
-        <v>0.001758312729255834</v>
+        <v>0.002338837983776767</v>
       </c>
       <c r="L34">
-        <v>0.0001413037151079847</v>
+        <v>0.0003151921108087671</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1821,31 +1821,31 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>-1.0935</v>
+        <v>0.9525</v>
       </c>
       <c r="E35">
         <v>217</v>
       </c>
       <c r="F35">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G35">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H35">
-        <v>472.2390905758871</v>
+        <v>484.1891081739</v>
       </c>
       <c r="I35">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J35">
-        <v>0.1813449036472676</v>
+        <v>0.2614612490896382</v>
       </c>
       <c r="K35">
-        <v>0.0006659500355209514</v>
+        <v>0.000588256986420227</v>
       </c>
       <c r="L35">
-        <v>6.038332251272069E-05</v>
+        <v>7.690320322756945E-05</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1856,34 +1856,34 @@
         <v>45</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>0.8034999999999999</v>
+        <v>0.9165</v>
       </c>
       <c r="E36">
         <v>415.73</v>
       </c>
       <c r="F36">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G36">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H36">
-        <v>534.2533445169266</v>
+        <v>485.2669650433398</v>
       </c>
       <c r="I36">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J36">
-        <v>0.3282105799802813</v>
+        <v>0.3100470809880271</v>
       </c>
       <c r="K36">
-        <v>0.0019195391203321</v>
+        <v>0.002318150217566029</v>
       </c>
       <c r="L36">
-        <v>0.0003150065239895187</v>
+        <v>0.0003593678541240536</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1894,34 +1894,34 @@
         <v>46</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>0.5565</v>
+        <v>-0.8195</v>
       </c>
       <c r="E37">
         <v>580.67</v>
       </c>
       <c r="F37">
-        <v>0.09282608695652177</v>
+        <v>0.1487857142857143</v>
       </c>
       <c r="G37">
-        <v>0.7604762741020793</v>
+        <v>0.770375918367347</v>
       </c>
       <c r="H37">
-        <v>526.1787421324054</v>
+        <v>537.2436185252153</v>
       </c>
       <c r="I37">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J37">
-        <v>0.3971711998187932</v>
+        <v>0.2473330447226253</v>
       </c>
       <c r="K37">
-        <v>0.002414757456861288</v>
+        <v>0.002463405936635873</v>
       </c>
       <c r="L37">
-        <v>0.0004795360582064879</v>
+        <v>0.0003046408453479705</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1935,31 +1935,31 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>-0.7004999999999999</v>
+        <v>0.8125</v>
       </c>
       <c r="E38">
         <v>457.35</v>
       </c>
       <c r="F38">
-        <v>0.09282608695652177</v>
+        <v>0.03069565217391306</v>
       </c>
       <c r="G38">
-        <v>0.7604762741020793</v>
+        <v>0.7512562769376181</v>
       </c>
       <c r="H38">
-        <v>485.0865348557124</v>
+        <v>488.3807737772771</v>
       </c>
       <c r="I38">
-        <v>24134.69076486111</v>
+        <v>24265.905834552</v>
       </c>
       <c r="J38">
-        <v>0.3024525731906079</v>
+        <v>0.3064405193975432</v>
       </c>
       <c r="K38">
-        <v>0.002527361871912881</v>
+        <v>0.002510701437664524</v>
       </c>
       <c r="L38">
-        <v>0.0003822035507719412</v>
+        <v>0.0003846903263050376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>